<commit_message>
txt file from list done.
</commit_message>
<xml_diff>
--- a/StudentRazorCRUD/wwwroot/Students.xlsx
+++ b/StudentRazorCRUD/wwwroot/Students.xlsx
@@ -6,13 +6,13 @@
     <workbookView tabRatio="600"/>
   </bookViews>
   <sheets>
-    <sheet name="Students" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -29,9 +29,6 @@
     <t xml:space="preserve">Subscribed</t>
   </si>
   <si>
-    <t xml:space="preserve">2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sohag</t>
   </si>
   <si>
@@ -39,12 +36,6 @@
   </si>
   <si>
     <t xml:space="preserve">01712262169</t>
-  </si>
-  <si>
-    <t xml:space="preserve">True</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4</t>
   </si>
   <si>
     <t xml:space="preserve">Rakib</t>
@@ -56,9 +47,6 @@
     <t xml:space="preserve">01683316263</t>
   </si>
   <si>
-    <t xml:space="preserve">5</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sajib</t>
   </si>
   <si>
@@ -66,9 +54,6 @@
   </si>
   <si>
     <t xml:space="preserve">01521015210</t>
-  </si>
-  <si>
-    <t xml:space="preserve">False</t>
   </si>
 </sst>
 </file>
@@ -136,54 +121,54 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
+      <c r="E2" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
+      <c r="E3" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
-        <v>14</v>
+      <c r="A4">
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
-      <c r="E4" t="s">
-        <v>18</v>
+      <c r="E4" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>